<commit_message>
Changed HRV frequency method from welch to lomb, added HF normalized and GSR peaks amplitude for analysis, corrected data issues, redid statistics
</commit_message>
<xml_diff>
--- a/Dec2021ExperimentResults/iMotionsData/BuzzwireParticipantComments.xlsx
+++ b/Dec2021ExperimentResults/iMotionsData/BuzzwireParticipantComments.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>GSR missing in post test</t>
+  </si>
+  <si>
+    <t>Participant ID was incorrectly entered as 2D2905 in MS Forms</t>
   </si>
 </sst>
 </file>
@@ -903,10 +906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1072,7 +1075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="1" customFormat="1">
+    <row r="17" spans="1:5" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1088,12 +1091,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8">
+    <row r="25" spans="1:5" ht="28.8">
       <c r="A25" s="7" t="s">
         <v>51</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="6" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="6" t="s">
         <v>59</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="1" customFormat="1">
+    <row r="30" spans="1:5" s="1" customFormat="1">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="6" t="s">
         <v>62</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="6" t="s">
         <v>64</v>
       </c>
@@ -1201,6 +1204,9 @@
       </c>
       <c r="D32" t="s">
         <v>75</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="28.8">

</xml_diff>